<commit_message>
add sdk integration notes, description of statistical indicators.
</commit_message>
<xml_diff>
--- a/docs/res/Clklog基础访问统计事件模板.xlsx
+++ b/docs/res/Clklog基础访问统计事件模板.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\至存相关\埋点系统\产品文档及交付\c++在ClkLog中实现用户访问统计功能的方案\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\至存相关\ClkLog\源码\clklog\docs\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409AF767-6761-4F52-A1F6-B6FEF904996B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108C9AEB-D3C5-4996-9D15-13697292A106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3053" yWindow="16103" windowWidth="22695" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="全埋点（预置）事件" sheetId="1" r:id="rId1"/>
+    <sheet name="ClkViewScreen事件" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -751,7 +751,7 @@
   <dimension ref="A1:BC430"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.765625" defaultRowHeight="20.05" customHeight="1"/>
@@ -945,7 +945,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>11</v>
@@ -979,7 +979,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>11</v>
@@ -1013,7 +1013,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>11</v>
@@ -1030,7 +1030,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>12</v>
@@ -1047,7 +1047,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>12</v>
@@ -1064,7 +1064,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>11</v>
@@ -1090,7 +1090,9 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:26" customFormat="1" ht="20.05" customHeight="1"/>
+    <row r="14" spans="1:26" customFormat="1" ht="20.05" customHeight="1">
+      <c r="E14" s="8"/>
+    </row>
     <row r="15" spans="1:26" customFormat="1" ht="20.05" customHeight="1"/>
     <row r="16" spans="1:26" customFormat="1" ht="20.05" customHeight="1"/>
     <row r="17" customFormat="1" ht="20.05" customHeight="1"/>
@@ -1518,7 +1520,7 @@
     <mergeCell ref="I4:I13"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="E4:E13">
+  <conditionalFormatting sqref="E4:E14">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>